<commit_message>
Update Possibility Filter V3.xlsx
</commit_message>
<xml_diff>
--- a/Downloads/Possibility Filter V3.xlsx
+++ b/Downloads/Possibility Filter V3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Tiny Magiq Client Work\1 - Hipoha Program Process\MVP Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E9D994-CA8F-4F12-B526-805803ED3EA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA81364-1329-4E04-BDE4-5F7B9C4BD89B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B3A634E3-7B0D-49A1-AC45-20D6757FFE73}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{B3A634E3-7B0D-49A1-AC45-20D6757FFE73}"/>
   </bookViews>
   <sheets>
     <sheet name="Listing out possibilities" sheetId="1" r:id="rId1"/>
@@ -32,8 +32,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={454A1C68-EB5F-4834-B639-9D142BA6BC9D}</author>
+    <author>tc={C3ADBBA1-F56B-4E9D-83EE-5A242512D345}</author>
+    <author>tc={825BD3C0-C530-4DA0-A8A6-C9C88D5CE162}</author>
+  </authors>
+  <commentList>
+    <comment ref="G6" authorId="0" shapeId="0" xr:uid="{454A1C68-EB5F-4834-B639-9D142BA6BC9D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Physical Location / Biz Area / Module / Process</t>
+      </text>
+    </comment>
+    <comment ref="H6" authorId="1" shapeId="0" xr:uid="{C3ADBBA1-F56B-4E9D-83EE-5A242512D345}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Skills / People / Money / Time</t>
+      </text>
+    </comment>
+    <comment ref="I6" authorId="2" shapeId="0" xr:uid="{825BD3C0-C530-4DA0-A8A6-C9C88D5CE162}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Clarity of implementation / Decomposable</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>ID</t>
   </si>
@@ -150,13 +186,16 @@
   </si>
   <si>
     <t>Possibility Filter V3</t>
+  </si>
+  <si>
+    <t>too hard to keep it running to get kids</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,9 +204,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFCC0099"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFCC0099"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -175,21 +221,77 @@
     <font>
       <b/>
       <sz val="20"/>
-      <color theme="1"/>
+      <color rgb="FF660033"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFCC0099"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFCC0099"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF660033"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF660033"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -221,41 +323,371 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="12">
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF660033"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF99FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF002060"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FFCC0099"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FFCC0099"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FFCC0099"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FFCC0099"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FFCC0099"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FFCC0099"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color rgb="FFCC0099"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF660033"/>
+      <color rgb="FFFF99FF"/>
+      <color rgb="FFCC0099"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -267,30 +699,36 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Anandan Kumaran" id="{5E6BA207-EE79-4484-A911-6D4840A56233}" userId="b67183372b1239e4" providerId="Windows Live"/>
+</personList>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{408707AA-3B5A-4F8A-BB1D-16E7E220C02C}" name="Table1" displayName="Table1" ref="B8:C20" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{408707AA-3B5A-4F8A-BB1D-16E7E220C02C}" name="Table1" displayName="Table1" ref="B6:C18" totalsRowShown="0" headerRowDxfId="4" dataDxfId="1">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{A1834E27-94EC-4053-8656-C0CB318E128C}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{D6C2D0AD-C2F2-4490-B0EB-51ECE27D70FE}" name="Possibilities" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{A1834E27-94EC-4053-8656-C0CB318E128C}" name="ID" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{D6C2D0AD-C2F2-4490-B0EB-51ECE27D70FE}" name="Possibilities" dataDxfId="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361E96DA-2FC8-4379-93F2-4D648DEA3C15}" name="Table2" displayName="Table2" ref="F8:K20" totalsRowShown="0">
-  <autoFilter ref="F8:K20" xr:uid="{4C205AB0-03C3-4750-A08C-35E222F1637D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{361E96DA-2FC8-4379-93F2-4D648DEA3C15}" name="Table2" displayName="Table2" ref="F6:K18" totalsRowShown="0" headerRowDxfId="0" dataDxfId="5">
+  <autoFilter ref="F6:K18" xr:uid="{4C205AB0-03C3-4750-A08C-35E222F1637D}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{2E4F7392-88D4-4459-B2E8-66DFB030D977}" name="IP"/>
-    <tableColumn id="2" xr3:uid="{4DCD6222-9668-4BE9-B0E8-A614070CB77C}" name="Where"/>
-    <tableColumn id="3" xr3:uid="{DFC55628-5C2D-426C-9D40-7F02EDA38FB4}" name="Resources"/>
-    <tableColumn id="4" xr3:uid="{3F4F6365-C778-4018-A452-6FAD76496835}" name="How"/>
-    <tableColumn id="5" xr3:uid="{41C8534F-B9D3-4A09-ACE1-1BDD1A45149B}" name="Total" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{2E4F7392-88D4-4459-B2E8-66DFB030D977}" name="IP" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{4DCD6222-9668-4BE9-B0E8-A614070CB77C}" name="Where" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{DFC55628-5C2D-426C-9D40-7F02EDA38FB4}" name="Resources" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{3F4F6365-C778-4018-A452-6FAD76496835}" name="How" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{41C8534F-B9D3-4A09-ACE1-1BDD1A45149B}" name="Total" dataDxfId="7">
       <calculatedColumnFormula>AVERAGE(Table2[[#This Row],[Where]:[How]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{BE700835-D18A-4DE3-A809-981BE1CE6788}" name="Comments"/>
+    <tableColumn id="6" xr3:uid="{BE700835-D18A-4DE3-A809-981BE1CE6788}" name="Comments" dataDxfId="6"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight17" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -589,406 +1027,488 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="G6" dT="2020-03-19T06:52:13.67" personId="{5E6BA207-EE79-4484-A911-6D4840A56233}" id="{454A1C68-EB5F-4834-B639-9D142BA6BC9D}">
+    <text>Physical Location / Biz Area / Module / Process</text>
+  </threadedComment>
+  <threadedComment ref="H6" dT="2020-03-19T06:53:01.25" personId="{5E6BA207-EE79-4484-A911-6D4840A56233}" id="{C3ADBBA1-F56B-4E9D-83EE-5A242512D345}">
+    <text>Skills / People / Money / Time</text>
+  </threadedComment>
+  <threadedComment ref="I6" dT="2020-03-19T06:52:23.20" personId="{5E6BA207-EE79-4484-A911-6D4840A56233}" id="{825BD3C0-C530-4DA0-A8A6-C9C88D5CE162}">
+    <text>Clarity of implementation / Decomposable</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F2573A-FEAE-4632-8EED-3B01D309CD71}">
-  <dimension ref="B2:K20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5F2573A-FEAE-4632-8EED-3B01D309CD71}">
+  <dimension ref="B1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="72" style="2" customWidth="1"/>
+    <col min="3" max="3" width="72" style="1" customWidth="1"/>
     <col min="4" max="4" width="4.42578125" customWidth="1"/>
     <col min="5" max="5" width="4.7109375" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" customWidth="1"/>
     <col min="10" max="10" width="8.42578125" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="11" max="11" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="4">
-        <v>3</v>
-      </c>
-      <c r="I2" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="3" t="s">
+      <c r="G2" s="19"/>
+      <c r="H2" s="13">
+        <v>3</v>
+      </c>
+      <c r="I2" s="14">
+        <v>3</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="5"/>
+      <c r="C3" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
       <c r="H3" s="4">
         <v>2</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="15">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="2" t="s">
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="5"/>
+      <c r="C4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="4">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="16">
         <v>1</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="17">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2" t="s">
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="5"/>
+      <c r="C5" s="12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="2:11" ht="5.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="3">
+        <v>3</v>
+      </c>
+      <c r="H7" s="3">
+        <v>3</v>
+      </c>
+      <c r="I7" s="3">
+        <v>3</v>
+      </c>
+      <c r="J7" s="3">
+        <f>AVERAGE(Table2[[#This Row],[Where]:[How]])</f>
+        <v>3</v>
+      </c>
+      <c r="K7" s="3"/>
+    </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3</v>
+      </c>
+      <c r="H8" s="3">
+        <v>3</v>
+      </c>
+      <c r="I8" s="3">
+        <v>3</v>
+      </c>
+      <c r="J8" s="3">
+        <f>AVERAGE(Table2[[#This Row],[Where]:[How]])</f>
+        <v>3</v>
+      </c>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="2:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="3">
+        <v>3</v>
+      </c>
+      <c r="H9" s="3">
         <v>1</v>
       </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" t="s">
-        <v>8</v>
-      </c>
-      <c r="J8" t="s">
-        <v>10</v>
-      </c>
-      <c r="K8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="I9" s="3">
+        <v>3</v>
+      </c>
+      <c r="J9" s="3">
+        <f>AVERAGE(Table2[[#This Row],[Where]:[How]])</f>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="3">
+        <v>3</v>
+      </c>
+      <c r="H10" s="3">
         <v>2</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
-      <c r="H9">
-        <v>3</v>
-      </c>
-      <c r="I9">
-        <v>3</v>
-      </c>
-      <c r="J9">
+      <c r="I10" s="3">
+        <v>3</v>
+      </c>
+      <c r="J10" s="3">
         <f>AVERAGE(Table2[[#This Row],[Where]:[How]])</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10">
-        <v>3</v>
-      </c>
-      <c r="H10">
-        <v>3</v>
-      </c>
-      <c r="I10">
-        <v>3</v>
-      </c>
-      <c r="J10">
-        <f>AVERAGE(Table2[[#This Row],[Where]:[How]])</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" t="s">
-        <v>4</v>
-      </c>
-      <c r="G11">
-        <v>3</v>
-      </c>
-      <c r="H11">
-        <v>3</v>
-      </c>
-      <c r="I11">
-        <v>3</v>
-      </c>
-      <c r="J11">
-        <f>AVERAGE(Table2[[#This Row],[Where]:[How]])</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12">
-        <v>3</v>
-      </c>
-      <c r="H12">
-        <v>3</v>
-      </c>
-      <c r="I12">
-        <v>3</v>
-      </c>
-      <c r="J12">
-        <f>AVERAGE(Table2[[#This Row],[Where]:[How]])</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F13" t="s">
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G13">
+      <c r="G11" s="3">
         <v>1</v>
       </c>
-      <c r="H13">
+      <c r="H11" s="3">
         <v>1</v>
       </c>
-      <c r="I13">
+      <c r="I11" s="3">
         <v>1</v>
       </c>
-      <c r="J13">
+      <c r="J11" s="3">
         <f>AVERAGE(Table2[[#This Row],[Where]:[How]])</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="K11" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F14" t="s">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G14">
+      <c r="G12" s="3">
         <v>1</v>
       </c>
-      <c r="H14">
+      <c r="H12" s="3">
         <v>1</v>
       </c>
-      <c r="I14">
+      <c r="I12" s="3">
         <v>1</v>
       </c>
-      <c r="J14">
+      <c r="J12" s="3">
         <f>AVERAGE(Table2[[#This Row],[Where]:[How]])</f>
         <v>1</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K12" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C13" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F15" t="s">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G15">
-        <v>3</v>
-      </c>
-      <c r="H15">
-        <v>3</v>
-      </c>
-      <c r="I15">
-        <v>3</v>
-      </c>
-      <c r="J15">
+      <c r="G13" s="3">
+        <v>3</v>
+      </c>
+      <c r="H13" s="3">
+        <v>3</v>
+      </c>
+      <c r="I13" s="3">
+        <v>3</v>
+      </c>
+      <c r="J13" s="3">
         <f>AVERAGE(Table2[[#This Row],[Where]:[How]])</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C14" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="F16" t="s">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G16">
+      <c r="G14" s="3">
         <v>0</v>
       </c>
-      <c r="H16">
+      <c r="H14" s="3">
         <v>0</v>
       </c>
-      <c r="I16">
+      <c r="I14" s="3">
         <v>0</v>
       </c>
-      <c r="J16">
+      <c r="J14" s="3">
         <f>AVERAGE(Table2[[#This Row],[Where]:[How]])</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C15" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F17" t="s">
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G17">
-        <v>3</v>
-      </c>
-      <c r="H17">
-        <v>3</v>
-      </c>
-      <c r="I17">
-        <v>3</v>
-      </c>
-      <c r="J17">
+      <c r="G15" s="3">
+        <v>3</v>
+      </c>
+      <c r="H15" s="3">
+        <v>3</v>
+      </c>
+      <c r="I15" s="3">
+        <v>3</v>
+      </c>
+      <c r="J15" s="3">
         <f>AVERAGE(Table2[[#This Row],[Where]:[How]])</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C16" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F18" t="s">
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G18">
+      <c r="G16" s="3">
         <v>0</v>
       </c>
-      <c r="H18">
+      <c r="H16" s="3">
         <v>0</v>
       </c>
-      <c r="I18">
+      <c r="I16" s="3">
         <v>0</v>
       </c>
-      <c r="J18">
+      <c r="J16" s="3">
         <f>AVERAGE(Table2[[#This Row],[Where]:[How]])</f>
         <v>0</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K16" s="3" t="s">
         <v>37</v>
       </c>
     </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="3">
+        <v>3</v>
+      </c>
+      <c r="H17" s="3">
+        <v>3</v>
+      </c>
+      <c r="I17" s="3">
+        <v>3</v>
+      </c>
+      <c r="J17" s="3">
+        <f>AVERAGE(Table2[[#This Row],[Where]:[How]])</f>
+        <v>3</v>
+      </c>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="3">
+        <v>3</v>
+      </c>
+      <c r="H18" s="3">
+        <v>3</v>
+      </c>
+      <c r="I18" s="3">
+        <v>3</v>
+      </c>
+      <c r="J18" s="3">
+        <f>AVERAGE(Table2[[#This Row],[Where]:[How]])</f>
+        <v>3</v>
+      </c>
+      <c r="K18" s="3"/>
+    </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" t="s">
-        <v>27</v>
-      </c>
-      <c r="G19">
-        <v>3</v>
-      </c>
-      <c r="H19">
-        <v>3</v>
-      </c>
-      <c r="I19">
-        <v>3</v>
-      </c>
-      <c r="J19">
-        <f>AVERAGE(Table2[[#This Row],[Where]:[How]])</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F20" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20">
-        <v>3</v>
-      </c>
-      <c r="H20">
-        <v>3</v>
-      </c>
-      <c r="I20">
-        <v>3</v>
-      </c>
-      <c r="J20">
-        <f>AVERAGE(Table2[[#This Row],[Where]:[How]])</f>
-        <v>3</v>
-      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F2:G4"/>
   </mergeCells>
-  <conditionalFormatting sqref="G9:J20">
+  <conditionalFormatting sqref="G7:J18">
     <cfRule type="iconSet" priority="2">
       <iconSet showValue="0">
         <cfvo type="percent" val="0"/>
@@ -1008,9 +1528,10 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="2">
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>